<commit_message>
add functions for various changes
</commit_message>
<xml_diff>
--- a/public/assets/app/reports/Acme Inc - System Inventory Report.xlsx
+++ b/public/assets/app/reports/Acme Inc - System Inventory Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>Material</t>
   </si>
@@ -47,37 +47,31 @@
     <t>PVC</t>
   </si>
   <si>
-    <t>HDPE</t>
-  </si>
-  <si>
     <t>PP</t>
   </si>
   <si>
-    <t>LDPE</t>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>Black chip</t>
+  </si>
+  <si>
+    <t>UV Stabilizer</t>
+  </si>
+  <si>
+    <t>red chip</t>
+  </si>
+  <si>
+    <t>blue chip</t>
+  </si>
+  <si>
+    <t>PSC</t>
+  </si>
+  <si>
+    <t>green ship</t>
   </si>
   <si>
     <t>Slip</t>
-  </si>
-  <si>
-    <t>PS</t>
-  </si>
-  <si>
-    <t>Black chip</t>
-  </si>
-  <si>
-    <t>UV Stabilizer</t>
-  </si>
-  <si>
-    <t>red chip</t>
-  </si>
-  <si>
-    <t>blue chip</t>
-  </si>
-  <si>
-    <t>PSC</t>
-  </si>
-  <si>
-    <t>green ship</t>
   </si>
 </sst>
 </file>
@@ -412,11 +406,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,22 +559,6 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20">
         <v>0</v>
       </c>
     </row>

</xml_diff>